<commit_message>
Rename assignment files and add .env
</commit_message>
<xml_diff>
--- a/02_activities/assignments/assignment_2_rubric_clean.xlsx
+++ b/02_activities/assignments/assignment_2_rubric_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCalderon\projects\dsi_production\assignments\responses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCalderon\projects\dsi_solutions\solutions\production\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0714DA9-59EC-42A1-BFC3-1A0B14AA635A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A8CED2-F4A6-4E77-9448-0CFD27A9D292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45960" yWindow="4920" windowWidth="29040" windowHeight="15720" xr2:uid="{C0852342-B4DD-4AAD-9E9C-10BBBB4B271E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{C0852342-B4DD-4AAD-9E9C-10BBBB4B271E}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">Rubric </t>
   </si>
@@ -56,94 +56,94 @@
     <t xml:space="preserve">Splits the data into fatures and target (X and Y) </t>
   </si>
   <si>
+    <t>Column Transformer</t>
+  </si>
+  <si>
+    <t>Model pipeline</t>
+  </si>
+  <si>
+    <t>Cross-validation</t>
+  </si>
+  <si>
+    <t>Performs cross validation using 5 folds</t>
+  </si>
+  <si>
+    <t>Student 1</t>
+  </si>
+  <si>
+    <t>Student 2</t>
+  </si>
+  <si>
+    <t>Student 3</t>
+  </si>
+  <si>
+    <t>Student 4</t>
+  </si>
+  <si>
+    <t>Student 5</t>
+  </si>
+  <si>
+    <t>Student 6</t>
+  </si>
+  <si>
+    <t>Student 7</t>
+  </si>
+  <si>
+    <t>Student 8</t>
+  </si>
+  <si>
+    <t>Student 9</t>
+  </si>
+  <si>
+    <t>Student 10</t>
+  </si>
+  <si>
     <t>- Creates a training and test set
-- Uses a 70-30% split
+- Uses a reasonable split
 - Sets the random state to 42.</t>
   </si>
   <si>
-    <t>- Explains what the random_state parameter does
-- Discusses its importance in reproducibility.</t>
-  </si>
-  <si>
-    <t>Column Transformer</t>
-  </si>
-  <si>
-    <t>Creates a ColumnTransformer object (regardless of the transforms)</t>
-  </si>
-  <si>
-    <t>Numerical transform: applies knn imputation with 7 neighbours and uses weights='distance'</t>
-  </si>
-  <si>
-    <t>Categorical transform: applies a simple imputer with "most_frequent" strategy and one-hot encoding with handle_unknown='infrequent_if_exists" and drop="if_binary"</t>
-  </si>
-  <si>
-    <t>Correctly applies the transforms to the required variables.</t>
-  </si>
-  <si>
-    <t>Model pipeline</t>
-  </si>
-  <si>
-    <t>Creates a model pipeline</t>
-  </si>
-  <si>
-    <t>Mode pipeline includes a RandomForestClassifier</t>
-  </si>
-  <si>
-    <t>Cross-validation</t>
-  </si>
-  <si>
-    <t>Performs cross validation using 5 folds</t>
-  </si>
-  <si>
-    <t>Returns training and validation scores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uses the required performance metrics (['neg_log_loss', 'roc_auc', 'accuracy', 'balanced_accuracy'])  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculates the mean performance metrics </t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Tests the model using the required performance metrics and the test set created above</t>
-  </si>
-  <si>
-    <t>Discussion on target recoding</t>
-  </si>
-  <si>
-    <t>Explains that ROC AUC requires that the label of interest is encoded as 1.</t>
-  </si>
-  <si>
-    <t>Student 1</t>
-  </si>
-  <si>
-    <t>Student 2</t>
-  </si>
-  <si>
-    <t>Student 3</t>
-  </si>
-  <si>
-    <t>Student 4</t>
-  </si>
-  <si>
-    <t>Student 5</t>
-  </si>
-  <si>
-    <t>Student 6</t>
-  </si>
-  <si>
-    <t>Student 7</t>
-  </si>
-  <si>
-    <t>Student 8</t>
-  </si>
-  <si>
-    <t>Student 9</t>
-  </si>
-  <si>
-    <t>Student 10</t>
+    <t xml:space="preserve">Creates  at least two different preprocessing steps. Generally, these should be column transformers, but a combination of pipelines and transformers can also be submitted. </t>
+  </si>
+  <si>
+    <t>The preprocessing pipelines treat month and day as categorical variables.</t>
+  </si>
+  <si>
+    <t>One hot encoding explicitly treats unseen values.</t>
+  </si>
+  <si>
+    <t>A non-linear transformation is applied in at least two pipelines.</t>
+  </si>
+  <si>
+    <t>Creates four pipelines in total.</t>
+  </si>
+  <si>
+    <t>Two models are linear (Linear Regression, Lasso, Ridge, etc.), another model is more complex (ensembles, MLP, etc)</t>
+  </si>
+  <si>
+    <t>Selects an ERROR metric (as opposed to R2 or variance explained)</t>
+  </si>
+  <si>
+    <t>Selects model based on optimal metric. 
+- Generally uses GridSearchCV and obtains the best params or best pipeline directly.</t>
+  </si>
+  <si>
+    <t>Grides include diversity with at least four cases per grid.
+- Hyperparams are reasonable (learning rate, regularization params, etc)</t>
+  </si>
+  <si>
+    <t>SHAP</t>
+  </si>
+  <si>
+    <t>Applies SHAP to obtain local and global explanation. 
+- Displays beeswarm and waterfall plots.</t>
+  </si>
+  <si>
+    <t>Interprets shap values and identifies variables with low importance.</t>
+  </si>
+  <si>
+    <t>Pickles pipeline and saves.
+- Ideally, uses a context manager (with statement).</t>
   </si>
 </sst>
 </file>
@@ -276,9 +276,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,7 +316,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -422,7 +422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -564,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -572,13 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5149F560-2317-43D9-AE63-996EC06808B6}">
-  <dimension ref="A2:L23"/>
+  <dimension ref="A2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -605,34 +605,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
@@ -656,7 +656,7 @@
     <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="10"/>
       <c r="B8" s="12" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -669,11 +669,9 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="10"/>
-      <c r="B9" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="B9" s="12"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -685,12 +683,12 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" s="8" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -706,7 +704,7 @@
     <row r="11" spans="1:12" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -719,10 +717,10 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" s="8" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -738,7 +736,7 @@
     <row r="13" spans="1:12" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -753,10 +751,10 @@
     </row>
     <row r="14" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -769,10 +767,10 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -785,28 +783,28 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="13"/>
+    <row r="16" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A16" s="10"/>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="B17" s="14" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -819,10 +817,10 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
     </row>
-    <row r="18" spans="1:12" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="13"/>
       <c r="B18" s="14" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -835,10 +833,10 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:12" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" s="16" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="13"/>
       <c r="B19" s="14" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -851,129 +849,143 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A21" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B22" s="1">
-        <f>COUNTA(B7:B21)</f>
+    <row r="20" spans="1:12" s="16" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="10"/>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B23" s="1">
+        <f>COUNTA(B7:B22)</f>
         <v>15</v>
       </c>
-      <c r="C22">
-        <f>SUM(C7:C21)</f>
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ref="D22:L22" si="0">SUM(D7:D21)</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
+      <c r="C23">
+        <f t="shared" ref="C23:L23" si="0">SUM(C7:C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22">
+      <c r="E23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="F23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22">
+      <c r="G23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22">
+      <c r="I23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22">
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L22">
+      <c r="K23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B23" s="11" t="s">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B24" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C23">
-        <f>IF(AND(C22&gt;=0, C22&lt;=1),C22/$B$22, "Error")</f>
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <f t="shared" ref="D23:L23" si="1">IF(AND(D22&gt;=0, D22&lt;=1),D22/$B$22, "Error")</f>
-        <v>0</v>
-      </c>
-      <c r="E23">
+      <c r="C24">
+        <f>IF(AND(C23&gt;=0, C23&lt;=1),C23/$B$23, "Error")</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:L24" si="1">IF(AND(D23&gt;=0, D23&lt;=1),D23/$B$23, "Error")</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J23">
+      <c r="J24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K23">
+      <c r="K24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>